<commit_message>
map to be merged
</commit_message>
<xml_diff>
--- a/map/bali-inner.xlsx
+++ b/map/bali-inner.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="3">
   <si>
     <t>O</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>o</t>
   </si>
 </sst>
 </file>
@@ -383,9 +380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DB1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="FG44" sqref="FG44"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BW53" sqref="BW53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3483,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="CG54" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK54" s="1" t="s">
         <v>1</v>
@@ -3530,10 +3527,10 @@
         <v>0</v>
       </c>
       <c r="CF55" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ55" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DS55" s="1" t="s">
         <v>1</v>
@@ -3565,22 +3562,22 @@
         <v>1</v>
       </c>
       <c r="BW56" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE56" s="1" t="s">
         <v>1</v>
       </c>
       <c r="CI56" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG56" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DH56" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DI56" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DJ56" s="1" t="s">
         <v>1</v>
@@ -3592,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="DT56" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DU56" s="1" t="s">
         <v>1</v>
@@ -3627,13 +3624,13 @@
         <v>1</v>
       </c>
       <c r="DF57" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DL57" s="1" t="s">
         <v>1</v>
       </c>
       <c r="DM57" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DN57" s="1" t="s">
         <v>0</v>
@@ -3683,13 +3680,13 @@
         <v>1</v>
       </c>
       <c r="CO58" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CP58" s="1" t="s">
         <v>1</v>
       </c>
       <c r="DE58" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DW58" s="1" t="s">
         <v>0</v>
@@ -3736,19 +3733,19 @@
         <v>0</v>
       </c>
       <c r="CM59" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CQ59" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB59" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DC59" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DD59" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DX59" s="1" t="s">
         <v>0</v>
@@ -3763,7 +3760,7 @@
         <v>1</v>
       </c>
       <c r="FP59" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GJ59" s="1" t="s">
         <v>0</v>
@@ -3786,52 +3783,52 @@
         <v>0</v>
       </c>
       <c r="CM60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CR60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="CS60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CT60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CU60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CV60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CW60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CX60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA60" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DY60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="DZ60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EA60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="EE60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EF60" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FO60" s="1" t="s">
         <v>0</v>
@@ -3848,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="BY61" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ61" s="1" t="s">
         <v>0</v>
@@ -3857,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="CB61" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF61" s="1" t="s">
         <v>0</v>
@@ -3943,9 +3940,6 @@
         <v>0</v>
       </c>
       <c r="CE62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="CF62" s="1" t="s">
         <v>1</v>
       </c>
       <c r="EM62" s="1" t="s">
@@ -4073,7 +4067,7 @@
         <v>0</v>
       </c>
       <c r="FK64" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GH64" s="1" t="s">
         <v>0</v>

</xml_diff>